<commit_message>
Adding 8.2 rerun files
</commit_message>
<xml_diff>
--- a/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Trial 8 Permutations/8.2/No constants/trial_8.2_NOconstant.xlsx
+++ b/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Trial 8 Permutations/8.2/No constants/trial_8.2_NOconstant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="765" windowWidth="18345" windowHeight="11745" tabRatio="877" activeTab="5"/>
+    <workbookView xWindow="765" yWindow="765" windowWidth="18345" windowHeight="11745" tabRatio="877" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="5" r:id="rId1"/>
@@ -1975,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2006,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -2023,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="4">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2031,10 +2031,10 @@
         <v>26</v>
       </c>
       <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
         <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>-2</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -2055,7 +2055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>